<commit_message>
fix(adminPanel): RN-1289: update the entity associated with a survey resubmission (#5817)
* Initial update

* test updates

* Update importSurveyResponses.js

* Update importSurveyResponses.js

* Update importSurveyResponses.js

* Update SurveyResponseUpdatePersistor.js

* Delete ~$nonPeriodicUpdates.xlsx

* test updates

* review comments

* review updates

* addition of tests

---------

Co-authored-by: Andrew <vanbeekandrew@gmail.com>
</commit_message>
<xml_diff>
--- a/packages/central-server/src/tests/testData/surveyResponses/functionality/nonPeriodicBaseline.xlsx
+++ b/packages/central-server/src/tests/testData/surveyResponses/functionality/nonPeriodicBaseline.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25003"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C16CBA87-E9F3-437D-B96C-8E7D9160C475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/salmanraza/Documents/GitHub/tupaia/packages/central-server/src/tests/testData/surveyResponses/functionality/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1C47B6-E64C-8341-A782-B331E591597C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16380" windowHeight="8200" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Clinic_Data" sheetId="1" r:id="rId1"/>
     <sheet name="Test_Facility_Fundamentals" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" iterateDelta="1E-4"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="82">
   <si>
     <t>Id</t>
   </si>
@@ -271,13 +276,19 @@
   </si>
   <si>
     <t>8000</t>
+  </si>
+  <si>
+    <t>Entity Code</t>
+  </si>
+  <si>
+    <t>Entity Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -330,9 +341,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -370,7 +381,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -476,7 +487,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -618,7 +629,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -632,27 +643,27 @@
       <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
-    <col min="6" max="6" width="37.875" customWidth="1"/>
-    <col min="7" max="7" width="27.625" customWidth="1"/>
+    <col min="6" max="6" width="37.83203125" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="25.625" customWidth="1"/>
-    <col min="10" max="10" width="14.625" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="21.375" customWidth="1"/>
-    <col min="13" max="13" width="16.625" customWidth="1"/>
-    <col min="14" max="14" width="25.625" customWidth="1"/>
-    <col min="15" max="15" width="27.875" customWidth="1"/>
+    <col min="12" max="12" width="21.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="25.6640625" customWidth="1"/>
+    <col min="15" max="15" width="27.83203125" customWidth="1"/>
     <col min="16" max="16" width="27" customWidth="1"/>
-    <col min="17" max="17" width="24.125" customWidth="1"/>
-    <col min="18" max="18" width="24.625" customWidth="1"/>
-    <col min="19" max="19" width="22.375" customWidth="1"/>
+    <col min="17" max="17" width="24.1640625" customWidth="1"/>
+    <col min="18" max="18" width="24.6640625" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +725,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -776,7 +787,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -838,7 +849,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -900,7 +911,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="25.35">
+    <row r="5" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -944,7 +955,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="25.35">
+    <row r="6" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>48</v>
       </c>
@@ -1000,7 +1011,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="25.35">
+    <row r="7" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>54</v>
       </c>
@@ -1056,7 +1067,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -1090,17 +1101,17 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="4" max="4" width="26.125" customWidth="1"/>
-    <col min="5" max="5" width="35.125" customWidth="1"/>
+    <col min="1" max="1" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1131,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1131,7 +1142,7 @@
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>80</v>
       </c>
       <c r="E2" t="s">
         <v>22</v>
@@ -1140,7 +1151,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -1151,7 +1162,7 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="E3" t="s">
         <v>27</v>
@@ -1160,7 +1171,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1180,7 +1191,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -1197,7 +1208,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>75</v>
       </c>

</xml_diff>